<commit_message>
allow blank lines in excel files
</commit_message>
<xml_diff>
--- a/test/services/data/foodDiary_standard_missing.xlsx
+++ b/test/services/data/foodDiary_standard_missing.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20181880\Desktop\sep\SEP-backend\src\services\food\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20181880\Desktop\sep\SEP-backend\test\services\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9A93A1-B060-444E-92EE-C1BE1721F266}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D591DF08-E88E-4B78-A809-340E13CDD4A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -326,10 +326,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -339,7 +339,7 @@
     <col min="8" max="8" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -365,7 +365,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>44325</v>
       </c>
@@ -388,7 +388,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>44324</v>
       </c>
@@ -408,7 +408,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="4">
         <v>0.96666666666666667</v>
@@ -446,34 +446,38 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="6">
-        <v>0.41736111111111113</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
+      <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="6">
-        <v>0.53541666666666665</v>
+        <v>0.41736111111111113</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
       <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6">
+        <v>0.53541666666666665</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8">
         <v>24</v>
       </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="H7">
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="H8">
         <v>4</v>
       </c>
     </row>

</xml_diff>